<commit_message>
if statement is removed in line segment finder
</commit_message>
<xml_diff>
--- a/Results/20221005 5miles-lineSegment_100clusters.xlsx
+++ b/Results/20221005 5miles-lineSegment_100clusters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3347DA-C5DA-4BB7-A55D-D6BE1484040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E936E823-86BA-4FE0-838E-8CA35891756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="$0M" sheetId="3" r:id="rId1"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF33C2D-0A39-4DCC-A04A-EA7B9F0D202F}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>152.16999999999999</v>
+        <v>126.59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -653,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>152.01</v>
+        <v>126.45</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -669,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>9.8800000000000008</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -685,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>7.28</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3650,7 +3650,7 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3698,7 +3698,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>332.99</v>
+        <v>306.77</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3714,7 +3714,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>332.64</v>
+        <v>306.41000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3730,7 +3730,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>24.73</v>
+        <v>11.23</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3738,7 +3738,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3746,7 +3746,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>19.14</v>
+        <v>5.74</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -6710,8 +6710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14A39EB-4C4E-4FCA-AF3D-76785108A3FD}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6759,7 +6759,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>332.07</v>
+        <v>300.22000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -6775,7 +6775,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>331.69</v>
+        <v>299.87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -6791,7 +6791,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>20.38</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -6799,7 +6799,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -6807,7 +6807,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>14.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>